<commit_message>
Commit before removing industrial equilibrium loop
</commit_message>
<xml_diff>
--- a/Data/UK time series data.xlsx
+++ b/Data/UK time series data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Modelling\Ventity\Urban1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59A2D99-741A-4682-AC84-67752EBFDB4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC0D993-B52A-4750-B373-0E5B34D19668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="0" windowWidth="20325" windowHeight="11745" xr2:uid="{B77BA640-AA93-49E8-8229-5CF7C9C7308D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B77BA640-AA93-49E8-8229-5CF7C9C7308D}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -33,27 +33,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Unemployment rate</t>
   </si>
   <si>
-    <t>UnemploymentData</t>
-  </si>
-  <si>
     <t>Population UK</t>
-  </si>
-  <si>
-    <t>PopulationData</t>
   </si>
   <si>
     <t>UKDataID</t>
   </si>
   <si>
     <t>Varname</t>
-  </si>
-  <si>
-    <t>GDPData</t>
   </si>
   <si>
     <t>GDP UK</t>
@@ -68,19 +59,16 @@
     <t>Industry GVA share</t>
   </si>
   <si>
-    <t>Agriculture share</t>
-  </si>
-  <si>
-    <t>Industry share</t>
-  </si>
-  <si>
-    <t>Services share</t>
-  </si>
-  <si>
     <t>IOPC</t>
   </si>
   <si>
     <t>SOPC</t>
+  </si>
+  <si>
+    <t>FIOC</t>
+  </si>
+  <si>
+    <t>BoE data</t>
   </si>
 </sst>
 </file>
@@ -460,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7A687D-A839-4303-8B50-84B2B3DAF972}">
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,65 +461,77 @@
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1900</v>
       </c>
@@ -547,22 +547,25 @@
       <c r="E3" s="4">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
+        <v>0.6480795886216052</v>
+      </c>
+      <c r="G3" s="3">
         <v>0.54659999999999997</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>0.38129999999999997</v>
       </c>
-      <c r="H3">
+      <c r="I3">
+        <f>H3*D3/C3*0.07*2.393758</f>
+        <v>265.17525799640731</v>
+      </c>
+      <c r="J3">
         <f>G3*D3/C3*0.07*2.393758</f>
-        <v>265.17525799640731</v>
-      </c>
-      <c r="I3">
-        <f>F3*D3/C3*0.07*2.393758</f>
         <v>380.13321799327622</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1901</v>
       </c>
@@ -578,22 +581,25 @@
       <c r="E4" s="4">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
+        <v>0.70611139818092794</v>
+      </c>
+      <c r="G4" s="3">
         <v>0.54659999999999997</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>0.38129999999999997</v>
       </c>
-      <c r="H4">
-        <f>G4*D4/C4*0.07*2.393758</f>
+      <c r="I4">
+        <f>H4*D4/C4*0.07*2.393758</f>
         <v>269.22711885742729</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I67" si="0">F4*D4/C4*0.07*2.393758</f>
+      <c r="J4">
+        <f t="shared" ref="J4:J67" si="0">G4*D4/C4*0.07*2.393758</f>
         <v>385.94162907807441</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1902</v>
       </c>
@@ -609,22 +615,25 @@
       <c r="E5" s="4">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
+        <v>0.69362147672977004</v>
+      </c>
+      <c r="G5" s="3">
         <v>0.54659999999999997</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>0.38129999999999997</v>
       </c>
-      <c r="H5">
-        <f t="shared" ref="H4:H67" si="1">G5*D5/C5*0.07*2.393758</f>
+      <c r="I5">
+        <f t="shared" ref="I5:I67" si="1">H5*D5/C5*0.07*2.393758</f>
         <v>270.42246406352126</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>387.65517665124764</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1903</v>
       </c>
@@ -640,22 +649,25 @@
       <c r="E6" s="4">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
+        <v>0.70897589941903383</v>
+      </c>
+      <c r="G6" s="3">
         <v>0.54659999999999997</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>0.38129999999999997</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f t="shared" si="1"/>
         <v>264.69705091953193</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>379.44770005931321</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1904</v>
       </c>
@@ -671,22 +683,25 @@
       <c r="E7" s="4">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
+        <v>0.7174744476015551</v>
+      </c>
+      <c r="G7" s="3">
         <v>0.54659999999999997</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>0.38129999999999997</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f t="shared" si="1"/>
         <v>265.85962655358412</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>381.11427189664073</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1905</v>
       </c>
@@ -702,22 +717,25 @@
       <c r="E8" s="4">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
+        <v>0.64844158551087128</v>
+      </c>
+      <c r="G8" s="3">
         <v>0.54659999999999997</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>0.38129999999999997</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" si="1"/>
         <v>272.35184885373025</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>390.4209823851271</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1906</v>
       </c>
@@ -733,22 +751,25 @@
       <c r="E9" s="4">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
+        <v>0.58972586199271648</v>
+      </c>
+      <c r="G9" s="3">
         <v>0.54659999999999997</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>0.38129999999999997</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="1"/>
         <v>276.25738433957514</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>396.01963356939888</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1907</v>
       </c>
@@ -764,22 +785,25 @@
       <c r="E10" s="2">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
+        <v>0.55851855848571053</v>
+      </c>
+      <c r="G10" s="1">
         <v>0.54659999999999997</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>0.38129999999999997</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f t="shared" si="1"/>
         <v>280.06472198077364</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>401.47751648227347</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1908</v>
       </c>
@@ -795,22 +819,25 @@
       <c r="E11" s="4">
         <v>7.1512423147410117E-2</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
+        <v>0.66495798366551995</v>
+      </c>
+      <c r="G11" s="3">
         <v>0.54115304160315159</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>0.38679749740647301</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <f t="shared" si="1"/>
         <v>269.92628787759702</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>377.64316644507079</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1909</v>
       </c>
@@ -826,22 +853,25 @@
       <c r="E12" s="4">
         <v>7.1424846294820224E-2</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
+        <v>0.64738900790244003</v>
+      </c>
+      <c r="G12" s="3">
         <v>0.5357060832063032</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>0.39229499481294611</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="1"/>
         <v>278.48536016212677</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>380.29111636737679</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1910</v>
       </c>
@@ -857,22 +887,25 @@
       <c r="E13" s="4">
         <v>7.1337269442230344E-2</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
+        <v>0.61681297339865837</v>
+      </c>
+      <c r="G13" s="3">
         <v>0.53025912480945503</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>0.39779249221941915</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <f t="shared" si="1"/>
         <v>287.74882301272754</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>383.57043443524054</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1911</v>
       </c>
@@ -888,22 +921,25 @@
       <c r="E14" s="4">
         <v>7.1249692589640451E-2</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
+        <v>0.60248414620920743</v>
+      </c>
+      <c r="G14" s="3">
         <v>0.52481216641260642</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>0.40328998962589219</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>299.42016045780832</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f t="shared" si="0"/>
         <v>389.64354960370156</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1912</v>
       </c>
@@ -919,22 +955,25 @@
       <c r="E15" s="4">
         <v>7.1162115737050571E-2</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
+        <v>0.59420695044603289</v>
+      </c>
+      <c r="G15" s="3">
         <v>0.51936520801575803</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>0.40878748703236528</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>307.06985787205326</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="0"/>
         <v>390.13278455967378</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1913</v>
       </c>
@@ -950,22 +989,25 @@
       <c r="E16" s="4">
         <v>7.1074538884460678E-2</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
+        <v>0.57369373598414697</v>
+      </c>
+      <c r="G16" s="3">
         <v>0.51391824961890964</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>0.41428498443883832</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>323.57883055043965</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>401.39776351166762</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1914</v>
       </c>
@@ -981,22 +1023,25 @@
       <c r="E17" s="4">
         <v>7.0986962031870798E-2</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
+        <v>0.66925828634811135</v>
+      </c>
+      <c r="G17" s="3">
         <v>0.50847129122206136</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>0.41978248184531142</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>332.35912319914513</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f t="shared" si="0"/>
         <v>402.57771543876777</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1915</v>
       </c>
@@ -1012,22 +1057,25 @@
       <c r="E18" s="4">
         <v>7.0899385179280905E-2</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
+        <v>1.1114328485162206</v>
+      </c>
+      <c r="G18" s="3">
         <v>0.50302433282521297</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>0.42527997925178446</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>356.05050900241082</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f t="shared" si="0"/>
         <v>421.13919883583071</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1916</v>
       </c>
@@ -1043,22 +1091,25 @@
       <c r="E19" s="4">
         <v>7.0811808326691025E-2</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
+        <v>1.0465471038380851</v>
+      </c>
+      <c r="G19" s="3">
         <v>0.49757737442836458</v>
       </c>
-      <c r="G19" s="3">
+      <c r="H19" s="3">
         <v>0.4307774766582575</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>366.26652050351601</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f t="shared" si="0"/>
         <v>423.06281894522272</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1917</v>
       </c>
@@ -1074,22 +1125,25 @@
       <c r="E20" s="4">
         <v>7.0724231474101132E-2</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20">
+        <v>0.98945748605150163</v>
+      </c>
+      <c r="G20" s="3">
         <v>0.49213041603151619</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>0.43627497406473059</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>373.17194420456627</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <f t="shared" si="0"/>
         <v>420.94842718490361</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1918</v>
       </c>
@@ -1105,22 +1159,25 @@
       <c r="E21" s="4">
         <v>7.0636654621511252E-2</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21">
+        <v>0.98531654935776836</v>
+      </c>
+      <c r="G21" s="3">
         <v>0.4866834576346678</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>0.44177247147120363</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>386.48353138631444</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f t="shared" si="0"/>
         <v>425.7737942510276</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1919</v>
       </c>
@@ -1136,22 +1193,25 @@
       <c r="E22" s="4">
         <v>7.0549077768921359E-2</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22">
+        <v>0.85525952691875951</v>
+      </c>
+      <c r="G22" s="3">
         <v>0.48123649923781942</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>0.44726996887767667</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <f t="shared" si="1"/>
         <v>353.199330087357</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <f t="shared" si="0"/>
         <v>380.02195759060288</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1920</v>
       </c>
@@ -1167,22 +1227,25 @@
       <c r="E23" s="4">
         <v>7.0461500916331479E-2</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23">
+        <v>0.75769471386012388</v>
+      </c>
+      <c r="G23" s="3">
         <v>0.47578954084097103</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="3">
         <v>0.45276746628414977</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <f t="shared" si="1"/>
         <v>327.85503934933473</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f t="shared" si="0"/>
         <v>344.52563457048734</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1921</v>
       </c>
@@ -1198,22 +1261,25 @@
       <c r="E24" s="1">
         <v>8.1347927144524962E-2</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24">
+        <v>0.80080408214870935</v>
+      </c>
+      <c r="G24" s="1">
         <v>0.5163543492224093</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>0.40112943385058869</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <f t="shared" si="1"/>
         <v>259.60025142229739</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f t="shared" si="0"/>
         <v>334.17073784484006</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1922</v>
       </c>
@@ -1229,22 +1295,25 @@
       <c r="E25" s="1">
         <v>5.9454306709426523E-2</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25">
+        <v>0.78105283318857166</v>
+      </c>
+      <c r="G25" s="1">
         <v>0.53630211358299029</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>0.40259059114668827</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <f t="shared" si="1"/>
         <v>274.16740252012073</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f t="shared" si="0"/>
         <v>365.22601541257785</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1923</v>
       </c>
@@ -1260,22 +1329,25 @@
       <c r="E26" s="1">
         <v>4.5592187579932067E-2</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26">
+        <v>0.80159262647952312</v>
+      </c>
+      <c r="G26" s="1">
         <v>0.54095898971245238</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>0.41186650353107163</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <f t="shared" si="1"/>
         <v>287.71359346468057</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <f t="shared" si="0"/>
         <v>377.89248096853572</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1924</v>
       </c>
@@ -1291,22 +1363,25 @@
       <c r="E27" s="1">
         <v>4.3742942222642626E-2</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27">
+        <v>0.7889262761317829</v>
+      </c>
+      <c r="G27" s="1">
         <v>0.53999055794618156</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>0.4149401129481185</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <f t="shared" si="1"/>
         <v>302.01481822435011</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <f t="shared" si="0"/>
         <v>393.03298262072946</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1925</v>
       </c>
@@ -1322,22 +1397,25 @@
       <c r="E28" s="1">
         <v>5.284224585824919E-2</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28">
+        <v>0.73936013831794878</v>
+      </c>
+      <c r="G28" s="1">
         <v>0.53984780903832952</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>0.40559994118223697</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <f t="shared" si="1"/>
         <v>305.03731290054316</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f t="shared" si="0"/>
         <v>406.00036717044122</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1926</v>
       </c>
@@ -1353,22 +1431,25 @@
       <c r="E29" s="1">
         <v>4.8896536946186682E-2</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29">
+        <v>0.80434990428522901</v>
+      </c>
+      <c r="G29" s="1">
         <v>0.56243427776679711</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>0.38695279745738603</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <f t="shared" si="1"/>
         <v>280.42753201908926</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <f t="shared" si="0"/>
         <v>407.60024859221056</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1927</v>
       </c>
@@ -1384,22 +1465,25 @@
       <c r="E30" s="1">
         <v>3.9346285082660512E-2</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30">
+        <v>0.72452885558871827</v>
+      </c>
+      <c r="G30" s="1">
         <v>0.56215710303729338</v>
       </c>
-      <c r="G30" s="2">
+      <c r="H30" s="2">
         <v>0.39699694828911963</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <f t="shared" si="1"/>
         <v>310.06828657220893</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <f t="shared" si="0"/>
         <v>439.06405445773919</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1928</v>
       </c>
@@ -1415,22 +1499,25 @@
       <c r="E31" s="1">
         <v>4.0491748423515682E-2</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31">
+        <v>0.73726582541027685</v>
+      </c>
+      <c r="G31" s="1">
         <v>0.57065115220117446</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>0.38702578144337074</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <f t="shared" si="1"/>
         <v>303.46448903201343</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <f t="shared" si="0"/>
         <v>447.44399112749426</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1929</v>
       </c>
@@ -1446,22 +1533,25 @@
       <c r="E32" s="1">
         <v>4.30900211552942E-2</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32">
+        <v>0.73029991013064299</v>
+      </c>
+      <c r="G32" s="1">
         <v>0.56541403420703507</v>
       </c>
-      <c r="G32" s="2">
+      <c r="H32" s="2">
         <v>0.38872214851733661</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <f t="shared" si="1"/>
         <v>313.10257161906588</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <f t="shared" si="0"/>
         <v>455.42192235500482</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1930</v>
       </c>
@@ -1477,22 +1567,25 @@
       <c r="E33" s="1">
         <v>5.4080676384680108E-2</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33">
+        <v>0.73611605623927989</v>
+      </c>
+      <c r="G33" s="1">
         <v>0.56458361294696213</v>
       </c>
-      <c r="G33" s="2">
+      <c r="H33" s="2">
         <v>0.3801964792388503</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <f t="shared" si="1"/>
         <v>302.43443711044068</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <f t="shared" si="0"/>
         <v>449.10864909962424</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1931</v>
       </c>
@@ -1508,22 +1601,25 @@
       <c r="E34" s="1">
         <v>4.3725363888051316E-2</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34">
+        <v>0.85310912285460272</v>
+      </c>
+      <c r="G34" s="1">
         <v>0.59255406924152298</v>
       </c>
-      <c r="G34" s="2">
+      <c r="H34" s="2">
         <v>0.36236767084235633</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <f t="shared" si="1"/>
         <v>272.83415729198936</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <f t="shared" si="0"/>
         <v>446.14628494764975</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1932</v>
       </c>
@@ -1539,22 +1635,25 @@
       <c r="E35" s="1">
         <v>4.1791764096235084E-2</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35">
+        <v>0.8574858979257034</v>
+      </c>
+      <c r="G35" s="1">
         <v>0.59728477754929765</v>
       </c>
-      <c r="G35" s="2">
+      <c r="H35" s="2">
         <v>0.359513001697426</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <f t="shared" si="1"/>
         <v>270.33129531079601</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <f t="shared" si="0"/>
         <v>449.12080181237661</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1933</v>
       </c>
@@ -1570,22 +1669,25 @@
       <c r="E36" s="1">
         <v>4.0490224112977508E-2</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36">
+        <v>0.83721003260747828</v>
+      </c>
+      <c r="G36" s="1">
         <v>0.59614851980176309</v>
       </c>
-      <c r="G36" s="2">
+      <c r="H36" s="2">
         <v>0.36161080654357264</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <f t="shared" si="1"/>
         <v>279.74892671131988</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <f t="shared" si="0"/>
         <v>461.19171650084496</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1934</v>
       </c>
@@ -1601,22 +1703,25 @@
       <c r="E37" s="1">
         <v>4.402022951464854E-2</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37">
+        <v>0.78113964044109507</v>
+      </c>
+      <c r="G37" s="1">
         <v>0.58145402062206097</v>
       </c>
-      <c r="G37" s="2">
+      <c r="H37" s="2">
         <v>0.37296260390982439</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <f t="shared" si="1"/>
         <v>305.47606860944649</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <f t="shared" si="0"/>
         <v>476.24154924585582</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1935</v>
       </c>
@@ -1632,22 +1737,25 @@
       <c r="E38" s="1">
         <v>3.9251998000769533E-2</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38">
+        <v>0.7720537240922688</v>
+      </c>
+      <c r="G38" s="1">
         <v>0.58185314683493661</v>
       </c>
-      <c r="G38" s="2">
+      <c r="H38" s="2">
         <v>0.37681918080738747</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <f t="shared" si="1"/>
         <v>318.60337193250274</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <f t="shared" si="0"/>
         <v>491.96108901342336</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1936</v>
       </c>
@@ -1663,22 +1771,25 @@
       <c r="E39" s="1">
         <v>3.5841513566875434E-2</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39">
+        <v>0.76650515029525212</v>
+      </c>
+      <c r="G39" s="1">
         <v>0.57543112939989638</v>
       </c>
-      <c r="G39" s="2">
+      <c r="H39" s="2">
         <v>0.38682609154493602</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <f t="shared" si="1"/>
         <v>341.59484109225787</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <f t="shared" si="0"/>
         <v>508.14645005418919</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1937</v>
       </c>
@@ -1694,22 +1805,25 @@
       <c r="E40" s="1">
         <v>3.0587314365164667E-2</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40">
+        <v>0.75054072438921571</v>
+      </c>
+      <c r="G40" s="1">
         <v>0.56953579347936623</v>
       </c>
-      <c r="G40" s="2">
+      <c r="H40" s="2">
         <v>0.39824683303444397</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <f t="shared" si="1"/>
         <v>362.27683173153434</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <f t="shared" si="0"/>
         <v>518.09482387412993</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1938</v>
       </c>
@@ -1725,22 +1839,25 @@
       <c r="E41" s="1">
         <v>4.1463310329682229E-2</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41">
+        <v>0.77186179238872088</v>
+      </c>
+      <c r="G41" s="1">
         <v>0.55718791309696791</v>
       </c>
-      <c r="G41" s="2">
+      <c r="H41" s="2">
         <v>0.39942988950927211</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <f t="shared" si="1"/>
         <v>364.17527139302734</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <f t="shared" si="0"/>
         <v>508.00920211128198</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1939</v>
       </c>
@@ -1756,22 +1873,25 @@
       <c r="E42" s="3">
         <v>4.3160573910298129E-2</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42">
+        <v>0.86290305617071417</v>
+      </c>
+      <c r="G42" s="3">
         <v>0.5522318494369044</v>
       </c>
-      <c r="G42" s="4">
+      <c r="H42" s="4">
         <v>0.40281911492936323</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <f t="shared" si="1"/>
         <v>382.16611647654116</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <f t="shared" si="0"/>
         <v>523.91828856226857</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1940</v>
       </c>
@@ -1787,22 +1907,25 @@
       <c r="E43" s="3">
         <v>4.4857837490914029E-2</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43">
+        <v>1.0899634088997714</v>
+      </c>
+      <c r="G43" s="3">
         <v>0.547275785776841</v>
       </c>
-      <c r="G43" s="4">
+      <c r="H43" s="4">
         <v>0.40620834034945441</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <f t="shared" si="1"/>
         <v>424.76198764267275</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <f t="shared" si="0"/>
         <v>572.27271689028669</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1941</v>
       </c>
@@ -1818,22 +1941,25 @@
       <c r="E44" s="3">
         <v>4.6555101071529929E-2</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44">
+        <v>1.104772609246258</v>
+      </c>
+      <c r="G44" s="3">
         <v>0.54231972211677748</v>
       </c>
-      <c r="G44" s="4">
+      <c r="H44" s="4">
         <v>0.40959756576954554</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <f t="shared" si="1"/>
         <v>467.99945209037696</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <f t="shared" si="0"/>
         <v>619.64560832194354</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1942</v>
       </c>
@@ -1849,22 +1975,25 @@
       <c r="E45" s="3">
         <v>4.8252364652145829E-2</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45">
+        <v>1.1147570913896014</v>
+      </c>
+      <c r="G45" s="3">
         <v>0.53736365845671408</v>
       </c>
-      <c r="G45" s="4">
+      <c r="H45" s="4">
         <v>0.41298679118963671</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <f t="shared" si="1"/>
         <v>479.64357347760318</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <f t="shared" si="0"/>
         <v>624.09508221008764</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1943</v>
       </c>
@@ -1880,22 +2009,25 @@
       <c r="E46" s="3">
         <v>4.9949628232761729E-2</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46">
+        <v>1.0913779185254497</v>
+      </c>
+      <c r="G46" s="3">
         <v>0.53240759479665056</v>
       </c>
-      <c r="G46" s="4">
+      <c r="H46" s="4">
         <v>0.41637601660972784</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <f t="shared" si="1"/>
         <v>488.30425352903677</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <f t="shared" si="0"/>
         <v>624.38008621915037</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1944</v>
       </c>
@@ -1911,22 +2043,25 @@
       <c r="E47" s="3">
         <v>5.1646891813377629E-2</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47">
+        <v>1.1708494569147663</v>
+      </c>
+      <c r="G47" s="3">
         <v>0.52745153113658705</v>
       </c>
-      <c r="G47" s="4">
+      <c r="H47" s="4">
         <v>0.41976524202981902</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <f t="shared" si="1"/>
         <v>466.22683721009605</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <f t="shared" si="0"/>
         <v>585.83235227933551</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1945</v>
       </c>
@@ -1942,22 +2077,25 @@
       <c r="E48" s="3">
         <v>5.334415539399353E-2</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48">
+        <v>1.1943352888034577</v>
+      </c>
+      <c r="G48" s="3">
         <v>0.52249546747652365</v>
       </c>
-      <c r="G48" s="4">
+      <c r="H48" s="4">
         <v>0.42315446744991014</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <f t="shared" si="1"/>
         <v>443.52636804006272</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <f t="shared" si="0"/>
         <v>547.64993597684031</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1946</v>
       </c>
@@ -1973,22 +2111,25 @@
       <c r="E49" s="3">
         <v>5.504141897460943E-2</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49">
+        <v>0.88399572438019269</v>
+      </c>
+      <c r="G49" s="3">
         <v>0.51753940381646013</v>
       </c>
-      <c r="G49" s="4">
+      <c r="H49" s="4">
         <v>0.42654369287000132</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <f t="shared" si="1"/>
         <v>433.6525525897506</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <f t="shared" si="0"/>
         <v>526.1648156621236</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1947</v>
       </c>
@@ -2004,22 +2145,25 @@
       <c r="E50" s="3">
         <v>5.673868255522533E-2</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50">
+        <v>0.7776221744606997</v>
+      </c>
+      <c r="G50" s="3">
         <v>0.51258334015639673</v>
       </c>
-      <c r="G50" s="4">
+      <c r="H50" s="4">
         <v>0.42993291829009245</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <f t="shared" si="1"/>
         <v>428.54584092522339</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <f t="shared" si="0"/>
         <v>510.9296106593215</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1948</v>
       </c>
@@ -2035,22 +2179,25 @@
       <c r="E51" s="1">
         <v>5.843594613584123E-2</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51">
+        <v>0.7339289973406925</v>
+      </c>
+      <c r="G51" s="1">
         <v>0.50762727649633321</v>
       </c>
-      <c r="G51" s="2">
+      <c r="H51" s="2">
         <v>0.43332214371018363</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <f t="shared" si="1"/>
         <v>443.29740120319053</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <f t="shared" si="0"/>
         <v>519.31306931127767</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1949</v>
       </c>
@@ -2066,22 +2213,25 @@
       <c r="E52" s="1">
         <v>6.0080305884217887E-2</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F52">
+        <v>0.73928649625009479</v>
+      </c>
+      <c r="G52" s="1">
         <v>0.49900760607765254</v>
       </c>
-      <c r="G52" s="1">
+      <c r="H52" s="1">
         <v>0.4403265504032563</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <f t="shared" si="1"/>
         <v>463.61674828954051</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <f t="shared" si="0"/>
         <v>525.40162179545553</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1950</v>
       </c>
@@ -2097,22 +2247,25 @@
       <c r="E53" s="1">
         <v>5.2263529607898922E-2</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F53">
+        <v>0.7261664479403106</v>
+      </c>
+      <c r="G53" s="1">
         <v>0.50793092681631669</v>
       </c>
-      <c r="G53" s="1">
+      <c r="H53" s="1">
         <v>0.43894642873257872</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <f t="shared" si="1"/>
         <v>475.55400544377443</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <f t="shared" si="0"/>
         <v>550.29172337435216</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1951</v>
       </c>
@@ -2128,22 +2281,25 @@
       <c r="E54" s="1">
         <v>4.635144125340683E-2</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F54">
+        <v>0.69912014297784109</v>
+      </c>
+      <c r="G54" s="1">
         <v>0.51024454203300951</v>
       </c>
-      <c r="G54" s="1">
+      <c r="H54" s="1">
         <v>0.44268655902967802</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <f t="shared" si="1"/>
         <v>499.89749400693296</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <f t="shared" si="0"/>
         <v>576.18638445247336</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1952</v>
       </c>
@@ -2159,22 +2315,25 @@
       <c r="E55" s="1">
         <v>5.3363213880874401E-2</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55">
+        <v>0.70212258280882334</v>
+      </c>
+      <c r="G55" s="1">
         <v>0.48089590785858477</v>
       </c>
-      <c r="G55" s="1">
+      <c r="H55" s="1">
         <v>0.46501234028046562</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <f t="shared" si="1"/>
         <v>534.442940499614</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <f t="shared" si="0"/>
         <v>552.69807015263439</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1953</v>
       </c>
@@ -2190,22 +2349,25 @@
       <c r="E56" s="1">
         <v>5.2832297899557082E-2</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F56">
+        <v>0.69631228190033545</v>
+      </c>
+      <c r="G56" s="1">
         <v>0.47295940392392199</v>
       </c>
-      <c r="G56" s="1">
+      <c r="H56" s="1">
         <v>0.47354354480978933</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <f t="shared" si="1"/>
         <v>573.78516398573811</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <f t="shared" si="0"/>
         <v>573.07736978674245</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1954</v>
       </c>
@@ -2221,22 +2383,25 @@
       <c r="E57" s="1">
         <v>4.9257052465809456E-2</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F57">
+        <v>0.7031340312570008</v>
+      </c>
+      <c r="G57" s="1">
         <v>0.47660022565986326</v>
       </c>
-      <c r="G57" s="1">
+      <c r="H57" s="1">
         <v>0.47335721475217629</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <f t="shared" si="1"/>
         <v>595.70423501698087</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <f t="shared" si="0"/>
         <v>599.78545586184919</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1955</v>
       </c>
@@ -2252,22 +2417,25 @@
       <c r="E58" s="1">
         <v>4.4955950372924332E-2</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F58">
+        <v>0.68410036412747677</v>
+      </c>
+      <c r="G58" s="1">
         <v>0.4761243834950622</v>
       </c>
-      <c r="G58" s="1">
+      <c r="H58" s="1">
         <v>0.47811107322113849</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <f t="shared" si="1"/>
         <v>622.54401914362813</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <f t="shared" si="0"/>
         <v>619.95716877321036</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1956</v>
       </c>
@@ -2283,22 +2451,25 @@
       <c r="E59" s="1">
         <v>4.3715351582428924E-2</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F59">
+        <v>0.63989134840182038</v>
+      </c>
+      <c r="G59" s="1">
         <v>0.48076365597089998</v>
       </c>
-      <c r="G59" s="1">
+      <c r="H59" s="1">
         <v>0.47455618125763094</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <f t="shared" si="1"/>
         <v>627.30297445053884</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <f t="shared" si="0"/>
         <v>635.50846729891077</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1957</v>
       </c>
@@ -2314,22 +2485,25 @@
       <c r="E60" s="1">
         <v>4.3376356297274175E-2</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F60">
+        <v>0.63189172166214358</v>
+      </c>
+      <c r="G60" s="1">
         <v>0.47986643309441601</v>
       </c>
-      <c r="G60" s="1">
+      <c r="H60" s="1">
         <v>0.47565272991125218</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <f t="shared" si="1"/>
         <v>637.87403407984016</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <f t="shared" si="0"/>
         <v>643.52482020769719</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1958</v>
       </c>
@@ -2345,22 +2519,25 @@
       <c r="E61" s="1">
         <v>4.2358486407335284E-2</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61">
+        <v>0.62720447150599112</v>
+      </c>
+      <c r="G61" s="1">
         <v>0.48167921916848611</v>
       </c>
-      <c r="G61" s="1">
+      <c r="H61" s="1">
         <v>0.47483340318346229</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <f t="shared" si="1"/>
         <v>640.01759060483084</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <f t="shared" si="0"/>
         <v>649.24491670085547</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1959</v>
       </c>
@@ -2376,22 +2553,25 @@
       <c r="E62" s="1">
         <v>4.0542671580320606E-2</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62">
+        <v>0.6406608348737548</v>
+      </c>
+      <c r="G62" s="1">
         <v>0.48587999058731668</v>
       </c>
-      <c r="G62" s="1">
+      <c r="H62" s="1">
         <v>0.47251625919781232</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <f t="shared" si="1"/>
         <v>656.42960498425691</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <f t="shared" si="0"/>
         <v>674.99478395189874</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1960</v>
       </c>
@@ -2407,22 +2587,25 @@
       <c r="E63" s="1">
         <v>3.8000013332828389E-2</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63">
+        <v>0.60886789268656061</v>
+      </c>
+      <c r="G63" s="1">
         <v>0.48804432134745157</v>
       </c>
-      <c r="G63" s="1">
+      <c r="H63" s="1">
         <v>0.47265137996428597</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <f t="shared" si="1"/>
         <v>693.69158047412395</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <f t="shared" si="0"/>
         <v>716.28318665337724</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1961</v>
       </c>
@@ -2438,22 +2621,25 @@
       <c r="E64" s="1">
         <v>3.741727678766478E-2</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F64">
+        <v>0.59252280976465843</v>
+      </c>
+      <c r="G64" s="1">
         <v>0.49424785146451816</v>
       </c>
-      <c r="G64" s="1">
+      <c r="H64" s="1">
         <v>0.46706402207707015</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <f t="shared" si="1"/>
         <v>699.14001614893641</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <f t="shared" si="0"/>
         <v>739.83101785018573</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1962</v>
       </c>
@@ -2469,22 +2655,25 @@
       <c r="E65" s="1">
         <v>3.8162233090138359E-2</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65">
+        <v>0.60956069667838009</v>
+      </c>
+      <c r="G65" s="1">
         <v>0.49873696837860459</v>
       </c>
-      <c r="G65" s="1">
+      <c r="H65" s="1">
         <v>0.46240286621493987</v>
       </c>
-      <c r="H65">
+      <c r="I65">
         <f t="shared" si="1"/>
         <v>694.38169298684875</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <f t="shared" si="0"/>
         <v>748.9439312793661</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1963</v>
       </c>
@@ -2500,22 +2689,25 @@
       <c r="E66" s="1">
         <v>3.5581401622627816E-2</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66">
+        <v>0.58604035759740469</v>
+      </c>
+      <c r="G66" s="1">
         <v>0.50631760615424815</v>
       </c>
-      <c r="G66" s="1">
+      <c r="H66" s="1">
         <v>0.45739317892313486</v>
       </c>
-      <c r="H66">
+      <c r="I66">
         <f t="shared" si="1"/>
         <v>694.74529437526417</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <f t="shared" si="0"/>
         <v>769.05776155906779</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1964</v>
       </c>
@@ -2531,22 +2723,25 @@
       <c r="E67" s="1">
         <v>3.5056921170389652E-2</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F67">
+        <v>0.55854298436134153</v>
+      </c>
+      <c r="G67" s="1">
         <v>0.50214175140202533</v>
       </c>
-      <c r="G67" s="1">
+      <c r="H67" s="1">
         <v>0.46197304962823921</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <f t="shared" si="1"/>
         <v>736.48159725830521</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <f t="shared" si="0"/>
         <v>800.51890347336928</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1965</v>
       </c>
@@ -2562,22 +2757,25 @@
       <c r="E68" s="1">
         <v>3.3206551319428762E-2</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F68">
+        <v>0.55328258794840246</v>
+      </c>
+      <c r="G68" s="1">
         <v>0.50702905207789517</v>
       </c>
-      <c r="G68" s="1">
+      <c r="H68" s="1">
         <v>0.45887648366737421</v>
       </c>
-      <c r="H68">
-        <f t="shared" ref="H68:H118" si="2">G68*D68/C68*0.07*2.393758</f>
+      <c r="I68">
+        <f t="shared" ref="I68:I118" si="2">H68*D68/C68*0.07*2.393758</f>
         <v>745.64939272545257</v>
       </c>
-      <c r="I68">
-        <f t="shared" ref="I68:I118" si="3">F68*D68/C68*0.07*2.393758</f>
+      <c r="J68">
+        <f t="shared" ref="J68:J118" si="3">G68*D68/C68*0.07*2.393758</f>
         <v>823.89470420125758</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1966</v>
       </c>
@@ -2593,22 +2791,25 @@
       <c r="E69" s="1">
         <v>3.3546993210739028E-2</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F69">
+        <v>0.54956055499138401</v>
+      </c>
+      <c r="G69" s="1">
         <v>0.51326609664347644</v>
       </c>
-      <c r="G69" s="1">
+      <c r="H69" s="1">
         <v>0.45231900958299809</v>
       </c>
-      <c r="H69">
+      <c r="I69">
         <f t="shared" si="2"/>
         <v>741.47824817057415</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <f t="shared" si="3"/>
         <v>841.38768904586561</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1967</v>
       </c>
@@ -2624,22 +2825,25 @@
       <c r="E70" s="1">
         <v>3.2681831315689726E-2</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F70">
+        <v>0.55715617104891213</v>
+      </c>
+      <c r="G70" s="1">
         <v>0.52301961946897901</v>
       </c>
-      <c r="G70" s="1">
+      <c r="H70" s="1">
         <v>0.44339730131843347</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <f t="shared" si="2"/>
         <v>738.33608705281051</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <f t="shared" si="3"/>
         <v>870.92153728117842</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1968</v>
       </c>
@@ -2655,22 +2859,25 @@
       <c r="E71" s="1">
         <v>3.1024134517640346E-2</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F71">
+        <v>0.52783335053790725</v>
+      </c>
+      <c r="G71" s="1">
         <v>0.52748720614166511</v>
       </c>
-      <c r="G71" s="1">
+      <c r="H71" s="1">
         <v>0.44085038751760997</v>
       </c>
-      <c r="H71">
+      <c r="I71">
         <f t="shared" si="2"/>
         <v>772.73765258785841</v>
       </c>
-      <c r="I71">
+      <c r="J71">
         <f t="shared" si="3"/>
         <v>924.59763444748216</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1969</v>
       </c>
@@ -2686,22 +2893,25 @@
       <c r="E72" s="1">
         <v>2.8676189469557748E-2</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F72">
+        <v>0.48355734902907782</v>
+      </c>
+      <c r="G72" s="1">
         <v>0.53543207479485466</v>
       </c>
-      <c r="G72" s="1">
+      <c r="H72" s="1">
         <v>0.43499425768226962</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <f t="shared" si="2"/>
         <v>775.01717311057678</v>
       </c>
-      <c r="I72">
+      <c r="J72">
         <f t="shared" si="3"/>
         <v>953.9644390049458</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1970</v>
       </c>
@@ -2717,22 +2927,25 @@
       <c r="E73" s="1">
         <v>2.8558102867502502E-2</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F73">
+        <v>0.41453605514388675</v>
+      </c>
+      <c r="G73" s="1">
         <v>0.55940260934914476</v>
       </c>
-      <c r="G73" s="1">
+      <c r="H73" s="1">
         <v>0.41203928778335275</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <f t="shared" si="2"/>
         <v>750.79171239532116</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <f t="shared" si="3"/>
         <v>1019.3077588574163</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1971</v>
       </c>
@@ -2748,22 +2961,25 @@
       <c r="E74" s="1">
         <v>2.8145696005453094E-2</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F74">
+        <v>0.41915758009558274</v>
+      </c>
+      <c r="G74" s="1">
         <v>0.56795705110888628</v>
       </c>
-      <c r="G74" s="1">
+      <c r="H74" s="1">
         <v>0.40389725288566053</v>
       </c>
-      <c r="H74">
+      <c r="I74">
         <f t="shared" si="2"/>
         <v>759.96218798236021</v>
       </c>
-      <c r="I74">
+      <c r="J74">
         <f t="shared" si="3"/>
         <v>1068.6526837133688</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1972</v>
       </c>
@@ -2779,22 +2995,25 @@
       <c r="E75" s="1">
         <v>2.7677484611850579E-2</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F75">
+        <v>0.44112097409926526</v>
+      </c>
+      <c r="G75" s="1">
         <v>0.5771644151329679</v>
       </c>
-      <c r="G75" s="1">
+      <c r="H75" s="1">
         <v>0.39515810025518161</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <f t="shared" si="2"/>
         <v>772.0487418376274</v>
       </c>
-      <c r="I75">
+      <c r="J75">
         <f t="shared" si="3"/>
         <v>1127.647542209316</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1973</v>
       </c>
@@ -2810,22 +3029,25 @@
       <c r="E76" s="1">
         <v>2.7222186539962768E-2</v>
       </c>
-      <c r="F76" s="1">
+      <c r="F76">
+        <v>0.4084360420131109</v>
+      </c>
+      <c r="G76" s="1">
         <v>0.58615379421301794</v>
       </c>
-      <c r="G76" s="1">
+      <c r="H76" s="1">
         <v>0.38662401924701933</v>
       </c>
-      <c r="H76">
+      <c r="I76">
         <f t="shared" si="2"/>
         <v>805.20095537715497</v>
       </c>
-      <c r="I76">
+      <c r="J76">
         <f t="shared" si="3"/>
         <v>1220.7508369952498</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1974</v>
       </c>
@@ -2841,22 +3063,25 @@
       <c r="E77" s="1">
         <v>2.673676125893908E-2</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F77">
+        <v>0.48969016021640993</v>
+      </c>
+      <c r="G77" s="1">
         <v>0.5957729036708137</v>
       </c>
-      <c r="G77" s="1">
+      <c r="H77" s="1">
         <v>0.37749033507024726</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <f t="shared" si="2"/>
         <v>768.11808632222562</v>
       </c>
-      <c r="I77">
+      <c r="J77">
         <f t="shared" si="3"/>
         <v>1212.2798920536648</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1975</v>
       </c>
@@ -2872,22 +3097,25 @@
       <c r="E78" s="1">
         <v>2.6376444424849748E-2</v>
       </c>
-      <c r="F78" s="1">
+      <c r="F78">
+        <v>0.5388470766123884</v>
+      </c>
+      <c r="G78" s="1">
         <v>0.60335397765836185</v>
       </c>
-      <c r="G78" s="1">
+      <c r="H78" s="1">
         <v>0.37026957791678833</v>
       </c>
-      <c r="H78">
+      <c r="I78">
         <f t="shared" si="2"/>
         <v>742.57728239480116</v>
       </c>
-      <c r="I78">
+      <c r="J78">
         <f t="shared" si="3"/>
         <v>1210.0290808993454</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1976</v>
       </c>
@@ -2903,22 +3131,25 @@
       <c r="E79" s="1">
         <v>2.5099464431022477E-2</v>
       </c>
-      <c r="F79" s="1">
+      <c r="F79">
+        <v>0.50361904308932792</v>
+      </c>
+      <c r="G79" s="1">
         <v>0.60323387982259447</v>
       </c>
-      <c r="G79" s="1">
+      <c r="H79" s="1">
         <v>0.37166665574638286</v>
       </c>
-      <c r="H79">
+      <c r="I79">
         <f t="shared" si="2"/>
         <v>767.96313725938353</v>
       </c>
-      <c r="I79">
+      <c r="J79">
         <f t="shared" si="3"/>
         <v>1246.4432191781793</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1977</v>
       </c>
@@ -2934,22 +3165,25 @@
       <c r="E80" s="1">
         <v>2.3870685244486597E-2</v>
       </c>
-      <c r="F80" s="1">
+      <c r="F80">
+        <v>0.46805992005065922</v>
+      </c>
+      <c r="G80" s="1">
         <v>0.60260551892371783</v>
       </c>
-      <c r="G80" s="1">
+      <c r="H80" s="1">
         <v>0.37352379583179562</v>
       </c>
-      <c r="H80">
+      <c r="I80">
         <f t="shared" si="2"/>
         <v>791.44161750135686</v>
       </c>
-      <c r="I80">
+      <c r="J80">
         <f t="shared" si="3"/>
         <v>1276.8318697077077</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1978</v>
       </c>
@@ -2965,22 +3199,25 @@
       <c r="E81" s="1">
         <v>2.2615911192448789E-2</v>
       </c>
-      <c r="F81" s="1">
+      <c r="F81">
+        <v>0.44303014041719857</v>
+      </c>
+      <c r="G81" s="1">
         <v>0.60250701455206968</v>
       </c>
-      <c r="G81" s="1">
+      <c r="H81" s="1">
         <v>0.3748770742554815</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <f t="shared" si="2"/>
         <v>823.16458069990006</v>
       </c>
-      <c r="I81">
+      <c r="J81">
         <f t="shared" si="3"/>
         <v>1323.000172756633</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1979</v>
       </c>
@@ -2996,22 +3233,25 @@
       <c r="E82" s="1">
         <v>2.1352591311603688E-2</v>
       </c>
-      <c r="F82" s="1">
+      <c r="F82">
+        <v>0.43879391420144609</v>
+      </c>
+      <c r="G82" s="1">
         <v>0.60282239956457406</v>
       </c>
-      <c r="G82" s="1">
+      <c r="H82" s="1">
         <v>0.37582500912382227</v>
       </c>
-      <c r="H82">
+      <c r="I82">
         <f t="shared" si="2"/>
         <v>852.46276106914502</v>
       </c>
-      <c r="I82">
+      <c r="J82">
         <f t="shared" si="3"/>
         <v>1367.3481931529361</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1980</v>
       </c>
@@ -3027,22 +3267,25 @@
       <c r="E83" s="1">
         <v>2.009477617859683E-2</v>
       </c>
-      <c r="F83" s="1">
+      <c r="F83">
+        <v>0.47605283753390981</v>
+      </c>
+      <c r="G83" s="1">
         <v>0.60313571655610199</v>
       </c>
-      <c r="G83" s="1">
+      <c r="H83" s="1">
         <v>0.37676950726530117</v>
       </c>
-      <c r="H83">
+      <c r="I83">
         <f t="shared" si="2"/>
         <v>836.39608840644996</v>
       </c>
-      <c r="I83">
+      <c r="J83">
         <f t="shared" si="3"/>
         <v>1338.9097163601693</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1981</v>
       </c>
@@ -3058,22 +3301,25 @@
       <c r="E84" s="1">
         <v>1.9188461635897106E-2</v>
       </c>
-      <c r="F84" s="1">
+      <c r="F84">
+        <v>0.47987316463702606</v>
+      </c>
+      <c r="G84" s="1">
         <v>0.61186628191038384</v>
       </c>
-      <c r="G84" s="1">
+      <c r="H84" s="1">
         <v>0.36894525645371901</v>
       </c>
-      <c r="H84">
+      <c r="I84">
         <f t="shared" si="2"/>
         <v>812.64999586011231</v>
       </c>
-      <c r="I84">
+      <c r="J84">
         <f t="shared" si="3"/>
         <v>1347.7152037155663</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1982</v>
       </c>
@@ -3089,22 +3335,25 @@
       <c r="E85" s="1">
         <v>1.8303683569838993E-2</v>
       </c>
-      <c r="F85" s="1">
+      <c r="F85">
+        <v>0.47157294518147608</v>
+      </c>
+      <c r="G85" s="1">
         <v>0.62021647845819405</v>
       </c>
-      <c r="G85" s="1">
+      <c r="H85" s="1">
         <v>0.36147983797196703</v>
       </c>
-      <c r="H85">
+      <c r="I85">
         <f t="shared" si="2"/>
         <v>814.0390530598454</v>
       </c>
-      <c r="I85">
+      <c r="J85">
         <f t="shared" si="3"/>
         <v>1396.704274431411</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1983</v>
       </c>
@@ -3120,22 +3369,25 @@
       <c r="E86" s="1">
         <v>1.7449030913496734E-2</v>
       </c>
-      <c r="F86" s="1">
+      <c r="F86">
+        <v>0.4484033364313198</v>
+      </c>
+      <c r="G86" s="1">
         <v>0.62812906068014518</v>
       </c>
-      <c r="G86" s="1">
+      <c r="H86" s="1">
         <v>0.35442190840635818</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <f t="shared" si="2"/>
         <v>830.44622407630209</v>
       </c>
-      <c r="I86">
+      <c r="J86">
         <f t="shared" si="3"/>
         <v>1471.7696460128402</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1984</v>
       </c>
@@ -3151,22 +3403,25 @@
       <c r="E87" s="1">
         <v>1.6673470901649005E-2</v>
       </c>
-      <c r="F87" s="1">
+      <c r="F87">
+        <v>0.43345569891561891</v>
+      </c>
+      <c r="G87" s="1">
         <v>0.63449551145417371</v>
       </c>
-      <c r="G87" s="1">
+      <c r="H87" s="1">
         <v>0.34883101764417723</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <f t="shared" si="2"/>
         <v>831.72577943791055</v>
       </c>
-      <c r="I87">
+      <c r="J87">
         <f t="shared" si="3"/>
         <v>1512.842170338138</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1985</v>
       </c>
@@ -3182,22 +3437,25 @@
       <c r="E88" s="1">
         <v>1.5951473325551517E-2</v>
       </c>
-      <c r="F88" s="1">
+      <c r="F88">
+        <v>0.41690274986603559</v>
+      </c>
+      <c r="G88" s="1">
         <v>0.63981802037233593</v>
       </c>
-      <c r="G88" s="1">
+      <c r="H88" s="1">
         <v>0.34423050630211266</v>
       </c>
-      <c r="H88">
+      <c r="I88">
         <f t="shared" si="2"/>
         <v>855.21463429566609</v>
       </c>
-      <c r="I88">
+      <c r="J88">
         <f t="shared" si="3"/>
         <v>1589.5794367169544</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1986</v>
       </c>
@@ -3213,22 +3471,25 @@
       <c r="E89" s="1">
         <v>1.6310743064405171E-2</v>
       </c>
-      <c r="F89" s="1">
+      <c r="F89">
+        <v>0.43154175336832234</v>
+      </c>
+      <c r="G89" s="1">
         <v>0.64632361778864478</v>
       </c>
-      <c r="G89" s="1">
+      <c r="H89" s="1">
         <v>0.33736563914695011</v>
       </c>
-      <c r="H89">
+      <c r="I89">
         <f t="shared" si="2"/>
         <v>859.83044722035925</v>
       </c>
-      <c r="I89">
+      <c r="J89">
         <f t="shared" si="3"/>
         <v>1647.2594148517476</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1987</v>
       </c>
@@ -3244,22 +3505,25 @@
       <c r="E90" s="1">
         <v>1.6689522664205356E-2</v>
       </c>
-      <c r="F90" s="1">
+      <c r="F90">
+        <v>0.39381876518473902</v>
+      </c>
+      <c r="G90" s="1">
         <v>0.65268957041654074</v>
       </c>
-      <c r="G90" s="1">
+      <c r="H90" s="1">
         <v>0.33062090691925389</v>
       </c>
-      <c r="H90">
+      <c r="I90">
         <f t="shared" si="2"/>
         <v>885.15406845670429</v>
       </c>
-      <c r="I90">
+      <c r="J90">
         <f t="shared" si="3"/>
         <v>1747.4116627311666</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1988</v>
       </c>
@@ -3275,22 +3539,25 @@
       <c r="E91" s="1">
         <v>1.7091262942630761E-2</v>
       </c>
-      <c r="F91" s="1">
+      <c r="F91">
+        <v>0.37204910267948893</v>
+      </c>
+      <c r="G91" s="1">
         <v>0.65900039252410025</v>
       </c>
-      <c r="G91" s="1">
+      <c r="H91" s="1">
         <v>0.32390834453326911</v>
       </c>
-      <c r="H91">
+      <c r="I91">
         <f t="shared" si="2"/>
         <v>914.77960684451989</v>
       </c>
-      <c r="I91">
+      <c r="J91">
         <f t="shared" si="3"/>
         <v>1861.1441482072166</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1989</v>
       </c>
@@ -3306,22 +3573,25 @@
       <c r="E92" s="1">
         <v>1.7536894279581959E-2</v>
       </c>
-      <c r="F92" s="1">
+      <c r="F92">
+        <v>0.33915996819860178</v>
+      </c>
+      <c r="G92" s="1">
         <v>0.66486552892260264</v>
       </c>
-      <c r="G92" s="1">
+      <c r="H92" s="1">
         <v>0.31759757679781558</v>
       </c>
-      <c r="H92">
+      <c r="I92">
         <f t="shared" si="2"/>
         <v>918.09798388099932</v>
       </c>
-      <c r="I92">
+      <c r="J92">
         <f t="shared" si="3"/>
         <v>1921.9658657673172</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1990</v>
       </c>
@@ -3337,22 +3607,25 @@
       <c r="E93" s="1">
         <v>1.6808704449797113E-2</v>
       </c>
-      <c r="F93" s="1">
+      <c r="F93">
+        <v>0.32709617327019769</v>
+      </c>
+      <c r="G93" s="1">
         <v>0.67829873300137178</v>
       </c>
-      <c r="G93" s="1">
+      <c r="H93" s="1">
         <v>0.30489256254883113</v>
       </c>
-      <c r="H93">
+      <c r="I93">
         <f t="shared" si="2"/>
         <v>886.3835962121932</v>
       </c>
-      <c r="I93">
+      <c r="J93">
         <f t="shared" si="3"/>
         <v>1971.9499394729826</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1991</v>
       </c>
@@ -3368,22 +3641,25 @@
       <c r="E94" s="1">
         <v>1.5960871761111998E-2</v>
       </c>
-      <c r="F94" s="1">
+      <c r="F94">
+        <v>0.32460079564031213</v>
+      </c>
+      <c r="G94" s="1">
         <v>0.69735563435984615</v>
       </c>
-      <c r="G94" s="1">
+      <c r="H94" s="1">
         <v>0.28668177228786923</v>
       </c>
-      <c r="H94">
+      <c r="I94">
         <f t="shared" si="2"/>
         <v>824.83443188702881</v>
       </c>
-      <c r="I94">
+      <c r="J94">
         <f t="shared" si="3"/>
         <v>2006.4161523071539</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1992</v>
       </c>
@@ -3399,22 +3675,25 @@
       <c r="E95" s="1">
         <v>1.626901933131962E-2</v>
       </c>
-      <c r="F95" s="1">
+      <c r="F95">
+        <v>0.34858257894374162</v>
+      </c>
+      <c r="G95" s="1">
         <v>0.70723187352825168</v>
       </c>
-      <c r="G95" s="1">
+      <c r="H95" s="1">
         <v>0.27650408288290934</v>
       </c>
-      <c r="H95">
+      <c r="I95">
         <f t="shared" si="2"/>
         <v>797.58760064097737</v>
       </c>
-      <c r="I95">
+      <c r="J95">
         <f t="shared" si="3"/>
         <v>2040.0399416275204</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1993</v>
       </c>
@@ -3430,22 +3709,25 @@
       <c r="E96" s="1">
         <v>1.6755687007230544E-2</v>
       </c>
-      <c r="F96" s="1">
+      <c r="F96">
+        <v>0.34225891608512676</v>
+      </c>
+      <c r="G96" s="1">
         <v>0.71289281691423356</v>
       </c>
-      <c r="G96" s="1">
+      <c r="H96" s="1">
         <v>0.27035307293596184</v>
       </c>
-      <c r="H96">
+      <c r="I96">
         <f t="shared" si="2"/>
         <v>798.58953244221141</v>
       </c>
-      <c r="I96">
+      <c r="J96">
         <f t="shared" si="3"/>
         <v>2105.7971901647302</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1994</v>
       </c>
@@ -3461,22 +3743,25 @@
       <c r="E97" s="1">
         <v>1.6369246063182942E-2</v>
       </c>
-      <c r="F97" s="1">
+      <c r="F97">
+        <v>0.32231346291016832</v>
+      </c>
+      <c r="G97" s="1">
         <v>0.70884806595997807</v>
       </c>
-      <c r="G97" s="1">
+      <c r="H97" s="1">
         <v>0.27478268797683902</v>
       </c>
-      <c r="H97">
+      <c r="I97">
         <f t="shared" si="2"/>
         <v>838.58965549116431</v>
       </c>
-      <c r="I97">
+      <c r="J97">
         <f t="shared" si="3"/>
         <v>2163.2827737643352</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1995</v>
       </c>
@@ -3492,22 +3777,25 @@
       <c r="E98" s="1">
         <v>1.7142734519508984E-2</v>
       </c>
-      <c r="F98" s="1">
+      <c r="F98">
+        <v>0.33757078740972812</v>
+      </c>
+      <c r="G98" s="1">
         <v>0.70593013021991258</v>
       </c>
-      <c r="G98" s="1">
+      <c r="H98" s="1">
         <v>0.27692145133003487</v>
       </c>
-      <c r="H98">
+      <c r="I98">
         <f t="shared" si="2"/>
         <v>861.0378294614718</v>
       </c>
-      <c r="I98">
+      <c r="J98">
         <f t="shared" si="3"/>
         <v>2194.9637493109667</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1996</v>
       </c>
@@ -3523,22 +3811,25 @@
       <c r="E99" s="1">
         <v>1.5748426500503163E-2</v>
       </c>
-      <c r="F99" s="1">
+      <c r="F99">
+        <v>0.3229649104991788</v>
+      </c>
+      <c r="G99" s="1">
         <v>0.70929739473114084</v>
       </c>
-      <c r="G99" s="1">
+      <c r="H99" s="1">
         <v>0.27496217154106811</v>
       </c>
-      <c r="H99">
+      <c r="I99">
         <f t="shared" si="2"/>
         <v>872.96232418180239</v>
       </c>
-      <c r="I99">
+      <c r="J99">
         <f t="shared" si="3"/>
         <v>2251.9094127393901</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1997</v>
       </c>
@@ -3554,22 +3845,25 @@
       <c r="E100" s="5">
         <v>1.1368194284747595E-2</v>
       </c>
-      <c r="F100" s="1">
+      <c r="F100">
+        <v>0.32307904628497119</v>
+      </c>
+      <c r="G100" s="1">
         <v>0.71911238148288892</v>
       </c>
-      <c r="G100" s="2">
+      <c r="H100" s="2">
         <v>0.26981540008449911</v>
       </c>
-      <c r="H100">
+      <c r="I100">
         <f t="shared" si="2"/>
         <v>879.12326587814073</v>
       </c>
-      <c r="I100">
+      <c r="J100">
         <f t="shared" si="3"/>
         <v>2343.0405571537422</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1998</v>
       </c>
@@ -3585,22 +3879,25 @@
       <c r="E101" s="5">
         <v>1.3936457578696429E-2</v>
       </c>
-      <c r="F101" s="1">
+      <c r="F101">
+        <v>0.27336557725008404</v>
+      </c>
+      <c r="G101" s="1">
         <v>0.73020743943401067</v>
       </c>
-      <c r="G101" s="2">
+      <c r="H101" s="2">
         <v>0.25974083390675146</v>
       </c>
-      <c r="H101">
+      <c r="I101">
         <f t="shared" si="2"/>
         <v>872.19547518979414</v>
       </c>
-      <c r="I101">
+      <c r="J101">
         <f t="shared" si="3"/>
         <v>2451.9965345645833</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1999</v>
       </c>
@@ -3616,22 +3913,25 @@
       <c r="E102" s="5">
         <v>1.1689565288905392E-2</v>
       </c>
-      <c r="F102" s="1">
+      <c r="F102">
+        <v>0.34155887558663817</v>
+      </c>
+      <c r="G102" s="1">
         <v>0.74186411311700307</v>
       </c>
-      <c r="G102" s="2">
+      <c r="H102" s="2">
         <v>0.2487098343362793</v>
       </c>
-      <c r="H102">
+      <c r="I102">
         <f t="shared" si="2"/>
         <v>860.62675663490938</v>
       </c>
-      <c r="I102">
+      <c r="J102">
         <f t="shared" si="3"/>
         <v>2567.1204648564494</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2000</v>
       </c>
@@ -3647,22 +3947,25 @@
       <c r="E103" s="5">
         <v>1.4249728678181077E-2</v>
       </c>
-      <c r="F103" s="1">
+      <c r="F103">
+        <v>0.3192656059738615</v>
+      </c>
+      <c r="G103" s="1">
         <v>0.73787984873175494</v>
       </c>
-      <c r="G103" s="2">
+      <c r="H103" s="2">
         <v>0.25343317367965584</v>
       </c>
-      <c r="H103">
+      <c r="I103">
         <f t="shared" si="2"/>
         <v>907.1694715693551</v>
       </c>
-      <c r="I103">
+      <c r="J103">
         <f t="shared" si="3"/>
         <v>2641.2567176457055</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2001</v>
       </c>
@@ -3678,22 +3981,25 @@
       <c r="E104" s="5">
         <v>1.2211438713500009E-2</v>
       </c>
-      <c r="F104" s="1">
+      <c r="F104">
+        <v>0.29999517561767064</v>
+      </c>
+      <c r="G104" s="1">
         <v>0.75212719762393776</v>
       </c>
-      <c r="G104" s="2">
+      <c r="H104" s="2">
         <v>0.23959951151215605</v>
       </c>
-      <c r="H104">
+      <c r="I104">
         <f t="shared" si="2"/>
         <v>875.35541369484963</v>
       </c>
-      <c r="I104">
+      <c r="J104">
         <f t="shared" si="3"/>
         <v>2747.8295346768573</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2002</v>
       </c>
@@ -3709,22 +4015,25 @@
       <c r="E105" s="5">
         <v>1.5157577215181581E-2</v>
       </c>
-      <c r="F105" s="1">
+      <c r="F105">
+        <v>0.28519393441207214</v>
+      </c>
+      <c r="G105" s="1">
         <v>0.75595316567949122</v>
       </c>
-      <c r="G105" s="2">
+      <c r="H105" s="2">
         <v>0.23601633226000729</v>
       </c>
-      <c r="H105">
+      <c r="I105">
         <f t="shared" si="2"/>
         <v>876.78449594416827</v>
       </c>
-      <c r="I105">
+      <c r="J105">
         <f t="shared" si="3"/>
         <v>2808.3141915683564</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2003</v>
       </c>
@@ -3740,22 +4049,25 @@
       <c r="E106" s="5">
         <v>1.2959656313913154E-2</v>
       </c>
-      <c r="F106" s="1">
+      <c r="F106">
+        <v>0.27003476418544575</v>
+      </c>
+      <c r="G106" s="1">
         <v>0.76532097143352895</v>
       </c>
-      <c r="G106" s="2">
+      <c r="H106" s="2">
         <v>0.22621614780615334</v>
       </c>
-      <c r="H106">
+      <c r="I106">
         <f t="shared" si="2"/>
         <v>866.2085205444854</v>
       </c>
-      <c r="I106">
+      <c r="J106">
         <f t="shared" si="3"/>
         <v>2930.5049742743131</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2004</v>
       </c>
@@ -3771,22 +4083,25 @@
       <c r="E107" s="5">
         <v>1.3492084606216002E-2</v>
       </c>
-      <c r="F107" s="1">
+      <c r="F107">
+        <v>0.2622845237852483</v>
+      </c>
+      <c r="G107" s="1">
         <v>0.77353929532825194</v>
       </c>
-      <c r="G107" s="2">
+      <c r="H107" s="2">
         <v>0.21789724013086931</v>
       </c>
-      <c r="H107">
+      <c r="I107">
         <f t="shared" si="2"/>
         <v>849.31449027770225</v>
       </c>
-      <c r="I107">
+      <c r="J107">
         <f t="shared" si="3"/>
         <v>3015.0823935489293</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2005</v>
       </c>
@@ -3802,22 +4117,25 @@
       <c r="E108" s="5">
         <v>1.1476745281557454E-2</v>
       </c>
-      <c r="F108" s="1">
+      <c r="F108">
+        <v>0.24091926540034331</v>
+      </c>
+      <c r="G108" s="1">
         <v>0.77334619618479028</v>
       </c>
-      <c r="G108" s="2">
+      <c r="H108" s="2">
         <v>0.22027767331632067</v>
       </c>
-      <c r="H108">
+      <c r="I108">
         <f t="shared" si="2"/>
         <v>880.10298589198328</v>
       </c>
-      <c r="I108">
+      <c r="J108">
         <f t="shared" si="3"/>
         <v>3089.8469470079203</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2006</v>
       </c>
@@ -3833,22 +4151,25 @@
       <c r="E109" s="5">
         <v>1.1207409699347439E-2</v>
       </c>
-      <c r="F109" s="1">
+      <c r="F109">
+        <v>0.26231770228847717</v>
+      </c>
+      <c r="G109" s="1">
         <v>0.77328845451098549</v>
       </c>
-      <c r="G109" s="2">
+      <c r="H109" s="2">
         <v>0.22051451454047905</v>
       </c>
-      <c r="H109">
+      <c r="I109">
         <f t="shared" si="2"/>
         <v>896.81104546988206</v>
       </c>
-      <c r="I109">
+      <c r="J109">
         <f t="shared" si="3"/>
         <v>3144.8888014692766</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2007</v>
       </c>
@@ -3864,22 +4185,25 @@
       <c r="E110" s="5">
         <v>9.5173433734786102E-3</v>
       </c>
-      <c r="F110" s="1">
+      <c r="F110">
+        <v>0.24104185834990891</v>
+      </c>
+      <c r="G110" s="1">
         <v>0.77829827818722619</v>
       </c>
-      <c r="G110" s="2">
+      <c r="H110" s="2">
         <v>0.21541748987830744</v>
       </c>
-      <c r="H110">
+      <c r="I110">
         <f t="shared" si="2"/>
         <v>891.06260238383118</v>
       </c>
-      <c r="I110">
+      <c r="J110">
         <f t="shared" si="3"/>
         <v>3219.3880338320732</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2008</v>
       </c>
@@ -3895,22 +4219,25 @@
       <c r="E111" s="5">
         <v>3.7359328637138296E-3</v>
       </c>
-      <c r="F111" s="1">
+      <c r="F111">
+        <v>0.35740023014945832</v>
+      </c>
+      <c r="G111" s="1">
         <v>0.78158795621547739</v>
       </c>
-      <c r="G111" s="2">
+      <c r="H111" s="2">
         <v>0.21144015269000152</v>
       </c>
-      <c r="H111">
+      <c r="I111">
         <f t="shared" si="2"/>
         <v>863.85303224127301</v>
       </c>
-      <c r="I111">
+      <c r="J111">
         <f t="shared" si="3"/>
         <v>3193.2304122476494</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2009</v>
       </c>
@@ -3926,22 +4253,25 @@
       <c r="E112" s="5">
         <v>8.3784138465887257E-3</v>
       </c>
-      <c r="F112" s="1">
+      <c r="F112">
+        <v>0.39317497619204939</v>
+      </c>
+      <c r="G112" s="1">
         <v>0.79457166648941668</v>
       </c>
-      <c r="G112" s="2">
+      <c r="H112" s="2">
         <v>0.19939677144669946</v>
       </c>
-      <c r="H112">
+      <c r="I112">
         <f t="shared" si="2"/>
         <v>771.93549780688841</v>
       </c>
-      <c r="I112">
+      <c r="J112">
         <f t="shared" si="3"/>
         <v>3076.0682355316512</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2010</v>
       </c>
@@ -3957,22 +4287,25 @@
       <c r="E113" s="5">
         <v>7.7799762111715994E-3</v>
       </c>
-      <c r="F113" s="1">
+      <c r="F113">
+        <v>0.33925223864010529</v>
+      </c>
+      <c r="G113" s="1">
         <v>0.79157026370759953</v>
       </c>
-      <c r="G113" s="2">
+      <c r="H113" s="2">
         <v>0.20112608552736219</v>
       </c>
-      <c r="H113">
+      <c r="I113">
         <f t="shared" si="2"/>
         <v>787.8337168516606</v>
       </c>
-      <c r="I113">
+      <c r="J113">
         <f t="shared" si="3"/>
         <v>3100.6706135150539</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2011</v>
       </c>
@@ -3988,22 +4321,25 @@
       <c r="E114" s="5">
         <v>7.4360360547683158E-3</v>
       </c>
-      <c r="F114" s="1">
+      <c r="F114">
+        <v>0.30296463797257989</v>
+      </c>
+      <c r="G114" s="1">
         <v>0.79014444846168419</v>
       </c>
-      <c r="G114" s="2">
+      <c r="H114" s="2">
         <v>0.20306664600657678</v>
       </c>
-      <c r="H114">
+      <c r="I114">
         <f t="shared" si="2"/>
         <v>800.43255660833972</v>
       </c>
-      <c r="I114">
+      <c r="J114">
         <f t="shared" si="3"/>
         <v>3114.5308863356549</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2012</v>
       </c>
@@ -4019,22 +4355,25 @@
       <c r="E115" s="5">
         <v>6.8132426143285409E-3</v>
       </c>
-      <c r="F115" s="1">
+      <c r="F115">
+        <v>0.37376197317470028</v>
+      </c>
+      <c r="G115" s="1">
         <v>0.79186213204812061</v>
       </c>
-      <c r="G115" s="2">
+      <c r="H115" s="2">
         <v>0.20146953414604138</v>
       </c>
-      <c r="H115">
+      <c r="I115">
         <f t="shared" si="2"/>
         <v>797.75766969285075</v>
       </c>
-      <c r="I115">
+      <c r="J115">
         <f t="shared" si="3"/>
         <v>3135.5315921999581</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2013</v>
       </c>
@@ -4050,22 +4389,25 @@
       <c r="E116" s="5">
         <v>5.4757652953274037E-3</v>
       </c>
-      <c r="F116" s="1">
+      <c r="F116">
+        <v>0.39445433661578017</v>
+      </c>
+      <c r="G116" s="1">
         <v>0.78782806645986314</v>
       </c>
-      <c r="G116" s="2">
+      <c r="H116" s="2">
         <v>0.20502232279528962</v>
       </c>
-      <c r="H116">
+      <c r="I116">
         <f t="shared" si="2"/>
         <v>818.83230317692937</v>
       </c>
-      <c r="I116">
+      <c r="J116">
         <f t="shared" si="3"/>
         <v>3146.4821067844114</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2014</v>
       </c>
@@ -4081,22 +4423,25 @@
       <c r="E117" s="5">
         <v>4.9220385637444818E-3</v>
       </c>
-      <c r="F117" s="1">
+      <c r="F117">
+        <v>0.35925101974799106</v>
+      </c>
+      <c r="G117" s="1">
         <v>0.79173798049100041</v>
       </c>
-      <c r="G117" s="2">
+      <c r="H117" s="2">
         <v>0.2014910027606146</v>
       </c>
-      <c r="H117">
+      <c r="I117">
         <f t="shared" si="2"/>
         <v>825.91385878704614</v>
       </c>
-      <c r="I117">
+      <c r="J117">
         <f t="shared" si="3"/>
         <v>3245.342777873178</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2015</v>
       </c>
@@ -4112,22 +4457,25 @@
       <c r="E118" s="5">
         <v>5.413950991066235E-3</v>
       </c>
-      <c r="F118" s="1">
+      <c r="F118">
+        <v>0.32083202653607018</v>
+      </c>
+      <c r="G118" s="1">
         <v>0.79814904456767111</v>
       </c>
-      <c r="G118" s="2">
+      <c r="H118" s="2">
         <v>0.19365357610149103</v>
       </c>
-      <c r="H118">
+      <c r="I118">
         <f t="shared" si="2"/>
         <v>806.73181186238583</v>
       </c>
-      <c r="I118">
+      <c r="J118">
         <f t="shared" si="3"/>
         <v>3324.9694522700415</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2016</v>
       </c>

</xml_diff>